<commit_message>
Added test data for ReplyAll
</commit_message>
<xml_diff>
--- a/Fulcrum_FluidTX_Trunk/src/com/proj/suiteTRANSMITTALS/testdata/TransmittalsTestData-IssuedForApproval.xlsx
+++ b/Fulcrum_FluidTX_Trunk/src/com/proj/suiteTRANSMITTALS/testdata/TransmittalsTestData-IssuedForApproval.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GITWS_Fluid_Sprint1\Fulcrum_FluidTX_Trunk\src\com\proj\suiteTRANSMITTALS\testdata\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git\Fulcrum_FluidTX_Trunk\src\com\proj\suiteTRANSMITTALS\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="30">
   <si>
     <t>To</t>
   </si>
@@ -103,6 +103,12 @@
   </si>
   <si>
     <t>AutoTestUser</t>
+  </si>
+  <si>
+    <t>Reply All- Message for New transmittal</t>
+  </si>
+  <si>
+    <t>ReplyAll</t>
   </si>
 </sst>
 </file>
@@ -503,9 +509,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O4"/>
+  <dimension ref="A1:O6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M12" sqref="M12"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
   <cols>
@@ -644,7 +652,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="1:15">
+    <row r="4" spans="1:15" ht="16.5" customHeight="1">
       <c r="A4" t="s">
         <v>26</v>
       </c>
@@ -686,6 +694,64 @@
       </c>
       <c r="O4" t="s">
         <v>17</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15">
+      <c r="A5" t="s">
+        <v>26</v>
+      </c>
+      <c r="B5" t="s">
+        <v>27</v>
+      </c>
+      <c r="C5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E5" t="s">
+        <v>13</v>
+      </c>
+      <c r="F5" t="s">
+        <v>14</v>
+      </c>
+      <c r="L5" t="s">
+        <v>28</v>
+      </c>
+      <c r="M5" t="s">
+        <v>29</v>
+      </c>
+      <c r="O5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15">
+      <c r="A6" t="s">
+        <v>26</v>
+      </c>
+      <c r="B6" t="s">
+        <v>27</v>
+      </c>
+      <c r="C6" t="s">
+        <v>6</v>
+      </c>
+      <c r="D6" t="s">
+        <v>8</v>
+      </c>
+      <c r="E6" t="s">
+        <v>13</v>
+      </c>
+      <c r="F6" t="s">
+        <v>14</v>
+      </c>
+      <c r="L6" t="s">
+        <v>28</v>
+      </c>
+      <c r="M6" t="s">
+        <v>29</v>
+      </c>
+      <c r="O6" t="s">
+        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Included Multi User test data
</commit_message>
<xml_diff>
--- a/Fulcrum_FluidTX_Trunk/src/com/proj/suiteTRANSMITTALS/testdata/TransmittalsTestData-IssuedForApproval.xlsx
+++ b/Fulcrum_FluidTX_Trunk/src/com/proj/suiteTRANSMITTALS/testdata/TransmittalsTestData-IssuedForApproval.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git\Fulcrum_FluidTX_Trunk\src\com\proj\suiteTRANSMITTALS\testdata\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\FluidTXGWS\Fulcrum_FluidTX_Trunk\src\com\proj\suiteTRANSMITTALS\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="31">
   <si>
     <t>To</t>
   </si>
@@ -109,6 +109,9 @@
   </si>
   <si>
     <t>ReplyAll</t>
+  </si>
+  <si>
+    <t>AutoTestAdmin@@AutoTestUser</t>
   </si>
 </sst>
 </file>
@@ -509,11 +512,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O6"/>
+  <dimension ref="A1:O8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M12" sqref="M12"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
   <cols>
@@ -754,6 +755,52 @@
         <v>18</v>
       </c>
     </row>
+    <row r="7" spans="1:15">
+      <c r="A7" t="s">
+        <v>30</v>
+      </c>
+      <c r="C7" t="s">
+        <v>6</v>
+      </c>
+      <c r="D7" t="s">
+        <v>8</v>
+      </c>
+      <c r="E7" t="s">
+        <v>13</v>
+      </c>
+      <c r="F7" t="s">
+        <v>14</v>
+      </c>
+      <c r="L7" t="s">
+        <v>5</v>
+      </c>
+      <c r="M7" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15">
+      <c r="A8" t="s">
+        <v>30</v>
+      </c>
+      <c r="C8" t="s">
+        <v>6</v>
+      </c>
+      <c r="D8" t="s">
+        <v>8</v>
+      </c>
+      <c r="E8" t="s">
+        <v>13</v>
+      </c>
+      <c r="F8" t="s">
+        <v>14</v>
+      </c>
+      <c r="L8" t="s">
+        <v>5</v>
+      </c>
+      <c r="M8" t="s">
+        <v>18</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>

</xml_diff>

<commit_message>
Changed ForwardTo from spinstall to AutoTestUser
</commit_message>
<xml_diff>
--- a/Fulcrum_FluidTX_Trunk/src/com/proj/suiteTRANSMITTALS/testdata/TransmittalsTestData-IssuedForApproval.xlsx
+++ b/Fulcrum_FluidTX_Trunk/src/com/proj/suiteTRANSMITTALS/testdata/TransmittalsTestData-IssuedForApproval.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="30">
   <si>
     <t>To</t>
   </si>
@@ -67,9 +67,6 @@
   </si>
   <si>
     <t>Forward</t>
-  </si>
-  <si>
-    <t>SPInstall</t>
   </si>
   <si>
     <t>Approved</t>
@@ -525,7 +522,7 @@
     <col min="6" max="11" width="20.42578125" customWidth="1"/>
     <col min="12" max="12" width="25.85546875" customWidth="1"/>
     <col min="13" max="13" width="19" customWidth="1"/>
-    <col min="14" max="14" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="13" customWidth="1"/>
     <col min="15" max="15" width="13.28515625" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="20.7109375" customWidth="1"/>
   </cols>
@@ -550,19 +547,19 @@
         <v>12</v>
       </c>
       <c r="G1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="J1" s="1" t="s">
-        <v>22</v>
-      </c>
       <c r="K1" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="L1" s="1" t="s">
         <v>4</v>
@@ -579,10 +576,10 @@
     </row>
     <row r="2" spans="1:15">
       <c r="A2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B2" t="s">
         <v>26</v>
-      </c>
-      <c r="B2" t="s">
-        <v>27</v>
       </c>
       <c r="C2" t="s">
         <v>6</v>
@@ -597,30 +594,30 @@
         <v>14</v>
       </c>
       <c r="G2" t="s">
+        <v>22</v>
+      </c>
+      <c r="H2" t="s">
         <v>23</v>
       </c>
-      <c r="H2" t="s">
-        <v>24</v>
-      </c>
       <c r="I2" t="s">
+        <v>22</v>
+      </c>
+      <c r="J2" t="s">
         <v>23</v>
-      </c>
-      <c r="J2" t="s">
-        <v>24</v>
       </c>
       <c r="L2" t="s">
         <v>5</v>
       </c>
       <c r="M2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="3" spans="1:15">
       <c r="A3" t="s">
+        <v>25</v>
+      </c>
+      <c r="B3" t="s">
         <v>26</v>
-      </c>
-      <c r="B3" t="s">
-        <v>27</v>
       </c>
       <c r="C3" t="s">
         <v>6</v>
@@ -635,30 +632,27 @@
         <v>14</v>
       </c>
       <c r="G3" t="s">
+        <v>22</v>
+      </c>
+      <c r="H3" t="s">
         <v>23</v>
       </c>
-      <c r="H3" t="s">
-        <v>24</v>
-      </c>
       <c r="I3" t="s">
+        <v>22</v>
+      </c>
+      <c r="J3" t="s">
         <v>23</v>
-      </c>
-      <c r="J3" t="s">
-        <v>24</v>
       </c>
       <c r="L3" t="s">
         <v>5</v>
       </c>
       <c r="M3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="4" spans="1:15" ht="16.5" customHeight="1">
       <c r="A4" t="s">
-        <v>26</v>
-      </c>
-      <c r="B4" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C4" t="s">
         <v>6</v>
@@ -673,16 +667,16 @@
         <v>14</v>
       </c>
       <c r="G4" t="s">
+        <v>22</v>
+      </c>
+      <c r="H4" t="s">
         <v>23</v>
       </c>
-      <c r="H4" t="s">
-        <v>24</v>
-      </c>
       <c r="I4" t="s">
+        <v>22</v>
+      </c>
+      <c r="J4" t="s">
         <v>23</v>
-      </c>
-      <c r="J4" t="s">
-        <v>24</v>
       </c>
       <c r="L4" t="s">
         <v>5</v>
@@ -691,18 +685,18 @@
         <v>15</v>
       </c>
       <c r="N4" t="s">
+        <v>26</v>
+      </c>
+      <c r="O4" t="s">
         <v>16</v>
-      </c>
-      <c r="O4" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="5" spans="1:15">
       <c r="A5" t="s">
+        <v>25</v>
+      </c>
+      <c r="B5" t="s">
         <v>26</v>
-      </c>
-      <c r="B5" t="s">
-        <v>27</v>
       </c>
       <c r="C5" t="s">
         <v>6</v>
@@ -717,21 +711,21 @@
         <v>14</v>
       </c>
       <c r="L5" t="s">
+        <v>27</v>
+      </c>
+      <c r="M5" t="s">
         <v>28</v>
       </c>
-      <c r="M5" t="s">
-        <v>29</v>
-      </c>
       <c r="O5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="6" spans="1:15">
       <c r="A6" t="s">
+        <v>25</v>
+      </c>
+      <c r="B6" t="s">
         <v>26</v>
-      </c>
-      <c r="B6" t="s">
-        <v>27</v>
       </c>
       <c r="C6" t="s">
         <v>6</v>
@@ -746,18 +740,18 @@
         <v>14</v>
       </c>
       <c r="L6" t="s">
+        <v>27</v>
+      </c>
+      <c r="M6" t="s">
         <v>28</v>
       </c>
-      <c r="M6" t="s">
-        <v>29</v>
-      </c>
       <c r="O6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="7" spans="1:15">
       <c r="A7" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C7" t="s">
         <v>6</v>
@@ -775,12 +769,12 @@
         <v>5</v>
       </c>
       <c r="M7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="8" spans="1:15">
       <c r="A8" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C8" t="s">
         <v>6</v>
@@ -798,7 +792,7 @@
         <v>5</v>
       </c>
       <c r="M8" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
1. Single User- Approve,Reject,Reply All 2. Multi User - Approve ,Reject test data
</commit_message>
<xml_diff>
--- a/Fulcrum_FluidTX_Trunk/src/com/proj/suiteTRANSMITTALS/testdata/TransmittalsTestData-IssuedForApproval.xlsx
+++ b/Fulcrum_FluidTX_Trunk/src/com/proj/suiteTRANSMITTALS/testdata/TransmittalsTestData-IssuedForApproval.xlsx
@@ -13,13 +13,14 @@
   </bookViews>
   <sheets>
     <sheet name="Transmittals_New" sheetId="1" r:id="rId1"/>
+    <sheet name="Transmittals_New_ActionRequired" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="30">
   <si>
     <t>To</t>
   </si>
@@ -800,4 +801,154 @@
   <pageSetup paperSize="9" orientation="portrait"/>
   <headerFooter alignWithMargins="0"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:O3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="28.42578125" customWidth="1"/>
+    <col min="2" max="2" width="20.85546875" customWidth="1"/>
+    <col min="3" max="3" width="21" customWidth="1"/>
+    <col min="4" max="5" width="13.28515625" customWidth="1"/>
+    <col min="6" max="11" width="20.42578125" customWidth="1"/>
+    <col min="12" max="12" width="25.85546875" customWidth="1"/>
+    <col min="13" max="13" width="19" customWidth="1"/>
+    <col min="14" max="14" width="13" customWidth="1"/>
+    <col min="15" max="15" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="20.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:15">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15">
+      <c r="A2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G2" t="s">
+        <v>22</v>
+      </c>
+      <c r="H2" t="s">
+        <v>23</v>
+      </c>
+      <c r="I2" t="s">
+        <v>22</v>
+      </c>
+      <c r="J2" t="s">
+        <v>23</v>
+      </c>
+      <c r="L2" t="s">
+        <v>5</v>
+      </c>
+      <c r="M2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15">
+      <c r="A3" t="s">
+        <v>25</v>
+      </c>
+      <c r="B3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E3" t="s">
+        <v>13</v>
+      </c>
+      <c r="F3" t="s">
+        <v>14</v>
+      </c>
+      <c r="G3" t="s">
+        <v>22</v>
+      </c>
+      <c r="H3" t="s">
+        <v>23</v>
+      </c>
+      <c r="I3" t="s">
+        <v>22</v>
+      </c>
+      <c r="J3" t="s">
+        <v>23</v>
+      </c>
+      <c r="L3" t="s">
+        <v>5</v>
+      </c>
+      <c r="M3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait"/>
+  <headerFooter alignWithMargins="0"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Test data for Delegate
</commit_message>
<xml_diff>
--- a/Fulcrum_FluidTX_Trunk/src/com/proj/suiteTRANSMITTALS/testdata/TransmittalsTestData-IssuedForApproval.xlsx
+++ b/Fulcrum_FluidTX_Trunk/src/com/proj/suiteTRANSMITTALS/testdata/TransmittalsTestData-IssuedForApproval.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\FluidTXGWS\Fulcrum_FluidTX_Trunk\src\com\proj\suiteTRANSMITTALS\testdata\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git\Fulcrum_FluidTX_Trunk\src\com\proj\suiteTRANSMITTALS\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="33">
   <si>
     <t>To</t>
   </si>
@@ -110,6 +110,15 @@
   </si>
   <si>
     <t>AutoTestAdmin@@AutoTestUser</t>
+  </si>
+  <si>
+    <t>DelegateTo</t>
+  </si>
+  <si>
+    <t>Delegate</t>
+  </si>
+  <si>
+    <t>Delegate- Message for New transmittal</t>
   </si>
 </sst>
 </file>
@@ -510,9 +519,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O8"/>
+  <dimension ref="A1:P9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="L12" sqref="L12"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
   <cols>
@@ -523,12 +534,12 @@
     <col min="6" max="11" width="20.42578125" customWidth="1"/>
     <col min="12" max="12" width="25.85546875" customWidth="1"/>
     <col min="13" max="13" width="19" customWidth="1"/>
-    <col min="14" max="14" width="13" customWidth="1"/>
-    <col min="15" max="15" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="20.7109375" customWidth="1"/>
+    <col min="14" max="15" width="13" customWidth="1"/>
+    <col min="16" max="16" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="20.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15">
+    <row r="1" spans="1:16">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -572,10 +583,13 @@
         <v>10</v>
       </c>
       <c r="O1" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="P1" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:15">
+    <row r="2" spans="1:16">
       <c r="A2" t="s">
         <v>25</v>
       </c>
@@ -613,7 +627,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:15">
+    <row r="3" spans="1:16">
       <c r="A3" t="s">
         <v>25</v>
       </c>
@@ -651,7 +665,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:15" ht="16.5" customHeight="1">
+    <row r="4" spans="1:16" ht="16.5" customHeight="1">
       <c r="A4" t="s">
         <v>25</v>
       </c>
@@ -688,11 +702,11 @@
       <c r="N4" t="s">
         <v>26</v>
       </c>
-      <c r="O4" t="s">
+      <c r="P4" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="5" spans="1:15">
+    <row r="5" spans="1:16">
       <c r="A5" t="s">
         <v>25</v>
       </c>
@@ -717,11 +731,11 @@
       <c r="M5" t="s">
         <v>28</v>
       </c>
-      <c r="O5" t="s">
+      <c r="P5" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="6" spans="1:15">
+    <row r="6" spans="1:16">
       <c r="A6" t="s">
         <v>25</v>
       </c>
@@ -746,11 +760,11 @@
       <c r="M6" t="s">
         <v>28</v>
       </c>
-      <c r="O6" t="s">
+      <c r="P6" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="7" spans="1:15">
+    <row r="7" spans="1:16">
       <c r="A7" t="s">
         <v>29</v>
       </c>
@@ -773,7 +787,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="8" spans="1:15">
+    <row r="8" spans="1:16">
       <c r="A8" t="s">
         <v>29</v>
       </c>
@@ -794,6 +808,35 @@
       </c>
       <c r="M8" t="s">
         <v>17</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16">
+      <c r="A9" t="s">
+        <v>25</v>
+      </c>
+      <c r="C9" t="s">
+        <v>6</v>
+      </c>
+      <c r="D9" t="s">
+        <v>8</v>
+      </c>
+      <c r="E9" t="s">
+        <v>13</v>
+      </c>
+      <c r="F9" t="s">
+        <v>14</v>
+      </c>
+      <c r="L9" t="s">
+        <v>32</v>
+      </c>
+      <c r="M9" t="s">
+        <v>31</v>
+      </c>
+      <c r="O9" t="s">
+        <v>26</v>
+      </c>
+      <c r="P9" t="s">
+        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated the test data as per latest Decision Table matrix(Sprint3)
</commit_message>
<xml_diff>
--- a/Fulcrum_FluidTX_Trunk/src/com/proj/suiteTRANSMITTALS/testdata/TransmittalsTestData-IssuedForApproval.xlsx
+++ b/Fulcrum_FluidTX_Trunk/src/com/proj/suiteTRANSMITTALS/testdata/TransmittalsTestData-IssuedForApproval.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git\Fulcrum_FluidTX_Trunk\src\com\proj\suiteTRANSMITTALS\testdata\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\FluidTXGWS\Fulcrum_FluidTX_Trunk\src\com\proj\suiteTRANSMITTALS\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -15,12 +15,12 @@
     <sheet name="Transmittals_New" sheetId="1" r:id="rId1"/>
     <sheet name="Transmittals_New_ActionRequired" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="30">
   <si>
     <t>To</t>
   </si>
@@ -110,15 +110,6 @@
   </si>
   <si>
     <t>AutoTestAdmin@@AutoTestUser</t>
-  </si>
-  <si>
-    <t>DelegateTo</t>
-  </si>
-  <si>
-    <t>Delegate</t>
-  </si>
-  <si>
-    <t>Delegate- Message for New transmittal</t>
   </si>
 </sst>
 </file>
@@ -519,11 +510,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P9"/>
+  <dimension ref="A1:O15"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="L12" sqref="L12"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
   <cols>
@@ -534,12 +523,12 @@
     <col min="6" max="11" width="20.42578125" customWidth="1"/>
     <col min="12" max="12" width="25.85546875" customWidth="1"/>
     <col min="13" max="13" width="19" customWidth="1"/>
-    <col min="14" max="15" width="13" customWidth="1"/>
-    <col min="16" max="16" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="20.7109375" customWidth="1"/>
+    <col min="14" max="14" width="13" customWidth="1"/>
+    <col min="15" max="15" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="20.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16">
+    <row r="1" spans="1:15">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -583,19 +572,13 @@
         <v>10</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="P1" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:16">
+    <row r="2" spans="1:15">
       <c r="A2" t="s">
         <v>25</v>
       </c>
-      <c r="B2" t="s">
-        <v>26</v>
-      </c>
       <c r="C2" t="s">
         <v>6</v>
       </c>
@@ -627,13 +610,10 @@
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:16">
+    <row r="3" spans="1:15">
       <c r="A3" t="s">
         <v>25</v>
       </c>
-      <c r="B3" t="s">
-        <v>26</v>
-      </c>
       <c r="C3" t="s">
         <v>6</v>
       </c>
@@ -665,7 +645,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:16" ht="16.5" customHeight="1">
+    <row r="4" spans="1:15">
       <c r="A4" t="s">
         <v>25</v>
       </c>
@@ -681,38 +661,17 @@
       <c r="F4" t="s">
         <v>14</v>
       </c>
-      <c r="G4" t="s">
-        <v>22</v>
-      </c>
-      <c r="H4" t="s">
-        <v>23</v>
-      </c>
-      <c r="I4" t="s">
-        <v>22</v>
-      </c>
-      <c r="J4" t="s">
-        <v>23</v>
-      </c>
       <c r="L4" t="s">
         <v>5</v>
       </c>
       <c r="M4" t="s">
-        <v>15</v>
-      </c>
-      <c r="N4" t="s">
-        <v>26</v>
-      </c>
-      <c r="P4" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="5" spans="1:16">
+    <row r="5" spans="1:15">
       <c r="A5" t="s">
         <v>25</v>
       </c>
-      <c r="B5" t="s">
-        <v>26</v>
-      </c>
       <c r="C5" t="s">
         <v>6</v>
       </c>
@@ -726,91 +685,124 @@
         <v>14</v>
       </c>
       <c r="L5" t="s">
-        <v>27</v>
+        <v>5</v>
       </c>
       <c r="M5" t="s">
-        <v>28</v>
-      </c>
-      <c r="P5" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="6" spans="1:16">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" ht="16.5" customHeight="1">
       <c r="A6" t="s">
         <v>25</v>
       </c>
-      <c r="B6" t="s">
+      <c r="C6" t="s">
+        <v>6</v>
+      </c>
+      <c r="D6" t="s">
+        <v>8</v>
+      </c>
+      <c r="E6" t="s">
+        <v>13</v>
+      </c>
+      <c r="F6" t="s">
+        <v>14</v>
+      </c>
+      <c r="G6" t="s">
+        <v>22</v>
+      </c>
+      <c r="H6" t="s">
+        <v>23</v>
+      </c>
+      <c r="I6" t="s">
+        <v>22</v>
+      </c>
+      <c r="J6" t="s">
+        <v>23</v>
+      </c>
+      <c r="L6" t="s">
+        <v>5</v>
+      </c>
+      <c r="M6" t="s">
+        <v>15</v>
+      </c>
+      <c r="N6" t="s">
         <v>26</v>
       </c>
-      <c r="C6" t="s">
-        <v>6</v>
-      </c>
-      <c r="D6" t="s">
-        <v>8</v>
-      </c>
-      <c r="E6" t="s">
-        <v>13</v>
-      </c>
-      <c r="F6" t="s">
-        <v>14</v>
-      </c>
-      <c r="L6" t="s">
-        <v>27</v>
-      </c>
-      <c r="M6" t="s">
-        <v>28</v>
-      </c>
-      <c r="P6" t="s">
+      <c r="O6" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" ht="16.5" customHeight="1">
+      <c r="A7" t="s">
+        <v>25</v>
+      </c>
+      <c r="C7" t="s">
+        <v>6</v>
+      </c>
+      <c r="D7" t="s">
+        <v>8</v>
+      </c>
+      <c r="E7" t="s">
+        <v>13</v>
+      </c>
+      <c r="F7" t="s">
+        <v>14</v>
+      </c>
+      <c r="G7" t="s">
+        <v>22</v>
+      </c>
+      <c r="H7" t="s">
+        <v>23</v>
+      </c>
+      <c r="I7" t="s">
+        <v>22</v>
+      </c>
+      <c r="J7" t="s">
+        <v>23</v>
+      </c>
+      <c r="L7" t="s">
+        <v>5</v>
+      </c>
+      <c r="M7" t="s">
+        <v>15</v>
+      </c>
+      <c r="N7" t="s">
+        <v>26</v>
+      </c>
+      <c r="O7" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="7" spans="1:16">
-      <c r="A7" t="s">
-        <v>29</v>
-      </c>
-      <c r="C7" t="s">
-        <v>6</v>
-      </c>
-      <c r="D7" t="s">
-        <v>8</v>
-      </c>
-      <c r="E7" t="s">
-        <v>13</v>
-      </c>
-      <c r="F7" t="s">
-        <v>14</v>
-      </c>
-      <c r="L7" t="s">
-        <v>5</v>
-      </c>
-      <c r="M7" t="s">
+    <row r="8" spans="1:15" ht="16.5" customHeight="1">
+      <c r="A8" t="s">
+        <v>25</v>
+      </c>
+      <c r="C8" t="s">
+        <v>6</v>
+      </c>
+      <c r="D8" t="s">
+        <v>8</v>
+      </c>
+      <c r="E8" t="s">
+        <v>13</v>
+      </c>
+      <c r="F8" t="s">
+        <v>14</v>
+      </c>
+      <c r="L8" t="s">
+        <v>5</v>
+      </c>
+      <c r="M8" t="s">
+        <v>15</v>
+      </c>
+      <c r="N8" t="s">
+        <v>26</v>
+      </c>
+      <c r="O8" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="8" spans="1:16">
-      <c r="A8" t="s">
-        <v>29</v>
-      </c>
-      <c r="C8" t="s">
-        <v>6</v>
-      </c>
-      <c r="D8" t="s">
-        <v>8</v>
-      </c>
-      <c r="E8" t="s">
-        <v>13</v>
-      </c>
-      <c r="F8" t="s">
-        <v>14</v>
-      </c>
-      <c r="L8" t="s">
-        <v>5</v>
-      </c>
-      <c r="M8" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="9" spans="1:16">
+    <row r="9" spans="1:15" ht="16.5" customHeight="1">
       <c r="A9" t="s">
         <v>25</v>
       </c>
@@ -827,16 +819,190 @@
         <v>14</v>
       </c>
       <c r="L9" t="s">
-        <v>32</v>
+        <v>5</v>
       </c>
       <c r="M9" t="s">
-        <v>31</v>
+        <v>15</v>
+      </c>
+      <c r="N9" t="s">
+        <v>26</v>
       </c>
       <c r="O9" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15">
+      <c r="A10" t="s">
+        <v>25</v>
+      </c>
+      <c r="B10" t="s">
         <v>26</v>
       </c>
-      <c r="P9" t="s">
+      <c r="C10" t="s">
+        <v>6</v>
+      </c>
+      <c r="D10" t="s">
+        <v>8</v>
+      </c>
+      <c r="E10" t="s">
+        <v>13</v>
+      </c>
+      <c r="F10" t="s">
+        <v>14</v>
+      </c>
+      <c r="L10" t="s">
+        <v>27</v>
+      </c>
+      <c r="M10" t="s">
+        <v>28</v>
+      </c>
+      <c r="O10" t="s">
         <v>16</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15">
+      <c r="A11" t="s">
+        <v>25</v>
+      </c>
+      <c r="B11" t="s">
+        <v>26</v>
+      </c>
+      <c r="C11" t="s">
+        <v>6</v>
+      </c>
+      <c r="D11" t="s">
+        <v>8</v>
+      </c>
+      <c r="E11" t="s">
+        <v>13</v>
+      </c>
+      <c r="F11" t="s">
+        <v>14</v>
+      </c>
+      <c r="L11" t="s">
+        <v>27</v>
+      </c>
+      <c r="M11" t="s">
+        <v>28</v>
+      </c>
+      <c r="O11" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15">
+      <c r="A12" t="s">
+        <v>29</v>
+      </c>
+      <c r="C12" t="s">
+        <v>6</v>
+      </c>
+      <c r="D12" t="s">
+        <v>8</v>
+      </c>
+      <c r="E12" t="s">
+        <v>13</v>
+      </c>
+      <c r="F12" t="s">
+        <v>14</v>
+      </c>
+      <c r="G12" t="s">
+        <v>22</v>
+      </c>
+      <c r="H12" t="s">
+        <v>23</v>
+      </c>
+      <c r="I12" t="s">
+        <v>22</v>
+      </c>
+      <c r="J12" t="s">
+        <v>23</v>
+      </c>
+      <c r="L12" t="s">
+        <v>5</v>
+      </c>
+      <c r="M12" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15">
+      <c r="A13" t="s">
+        <v>29</v>
+      </c>
+      <c r="C13" t="s">
+        <v>6</v>
+      </c>
+      <c r="D13" t="s">
+        <v>8</v>
+      </c>
+      <c r="E13" t="s">
+        <v>13</v>
+      </c>
+      <c r="F13" t="s">
+        <v>14</v>
+      </c>
+      <c r="G13" t="s">
+        <v>22</v>
+      </c>
+      <c r="H13" t="s">
+        <v>23</v>
+      </c>
+      <c r="I13" t="s">
+        <v>22</v>
+      </c>
+      <c r="J13" t="s">
+        <v>23</v>
+      </c>
+      <c r="L13" t="s">
+        <v>5</v>
+      </c>
+      <c r="M13" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15">
+      <c r="A14" t="s">
+        <v>29</v>
+      </c>
+      <c r="C14" t="s">
+        <v>6</v>
+      </c>
+      <c r="D14" t="s">
+        <v>8</v>
+      </c>
+      <c r="E14" t="s">
+        <v>13</v>
+      </c>
+      <c r="F14" t="s">
+        <v>14</v>
+      </c>
+      <c r="L14" t="s">
+        <v>5</v>
+      </c>
+      <c r="M14" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15">
+      <c r="A15" t="s">
+        <v>29</v>
+      </c>
+      <c r="C15" t="s">
+        <v>6</v>
+      </c>
+      <c r="D15" t="s">
+        <v>8</v>
+      </c>
+      <c r="E15" t="s">
+        <v>13</v>
+      </c>
+      <c r="F15" t="s">
+        <v>14</v>
+      </c>
+      <c r="L15" t="s">
+        <v>5</v>
+      </c>
+      <c r="M15" t="s">
+        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>